<commit_message>
Lab #7 et al.
</commit_message>
<xml_diff>
--- a/register/2018.xlsx
+++ b/register/2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\nets\register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A5A8AC-96CA-4288-9F26-8441548217DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB2446C-2C64-4182-B5CA-55CA986DC5E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11715" activeTab="1" xr2:uid="{0773F02F-154F-49AB-B554-199499201140}"/>
   </bookViews>
@@ -89,6 +89,82 @@
           </rPr>
           <t xml:space="preserve">
 Неверный шлюз на сервере</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{579E65D6-3ED6-426B-936B-D6ABDDDA5178}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Неверный шлюз в средней сети
+Не включён DHCP на 1 машине
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{D94D48B2-12A8-46F8-B959-0E6B49D413F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DHCP настроен не правильно
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{1203290A-15C7-44A3-AD37-A1E5D30E81C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Одинаковый router-id
+</t>
         </r>
       </text>
     </comment>
@@ -253,6 +329,31 @@
     <author>С.С. Уколов</author>
   </authors>
   <commentList>
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{95598E74-3CF2-4CEE-B296-03695DC5D2D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Опечатки в настройке IP правой подсети
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E8" authorId="0" shapeId="0" xr:uid="{F8D4EFFC-B078-4504-B1E4-DC66729E414D}">
       <text>
         <r>
@@ -300,6 +401,31 @@
           </rPr>
           <t xml:space="preserve">
 Глупо чужой IP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{0FA34685-E1CC-4AF1-83E5-F806BEF9537D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Не включён OSPF на портах правого маршрутизатора
+</t>
         </r>
       </text>
     </comment>
@@ -468,6 +594,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{A5DA5D4C-F236-4E2D-B8D9-AC258C4E120F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Маршрутизатор совсем не настроен
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E23" authorId="0" shapeId="0" xr:uid="{EDE0AB72-0393-43FB-B884-B38D58C2EC24}">
       <text>
         <r>
@@ -517,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{503CB5C0-C787-4635-A6E8-6E1D256D4A32}">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{7A7FBE6E-DA8A-454E-8665-824D31AA9FB5}">
       <text>
         <r>
           <rPr>
@@ -537,11 +688,37 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Чужой IP</t>
+Опечатки в IP в правой подсети
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="G27" authorId="0" shapeId="0" xr:uid="{E6B374B0-D564-4684-AD8A-A839CF12FB49}">
+    <comment ref="K24" authorId="0" shapeId="0" xr:uid="{D4E636B1-C818-4EED-8ACA-B620F5B91088}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DHCP настроен на Windows, не на Cisco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{503CB5C0-C787-4635-A6E8-6E1D256D4A32}">
       <text>
         <r>
           <rPr>
@@ -729,7 +906,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="226">
   <si>
     <t/>
   </si>
@@ -1967,8 +2144,8 @@
   </sheetPr>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18443,7 +18620,9 @@
       <c r="J5" s="7">
         <v>43438</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>43445</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -18621,8 +18800,8 @@
       <c r="J8" s="2">
         <v>4</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>0</v>
+      <c r="K8" s="2">
+        <v>3</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>0</v>
@@ -18807,26 +18986,23 @@
       <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>0</v>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>0</v>
@@ -18961,8 +19137,8 @@
       <c r="J13" s="2">
         <v>5</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>0</v>
+      <c r="K13" s="2">
+        <v>5</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>0</v>
@@ -19092,11 +19268,11 @@
       <c r="I15" s="2">
         <v>5</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>0</v>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>0</v>
@@ -19163,9 +19339,7 @@
       <c r="J16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
         <v>0</v>
       </c>
@@ -19231,8 +19405,8 @@
       <c r="J17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>0</v>
+      <c r="K17" s="2">
+        <v>5</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>0</v>
@@ -19299,8 +19473,8 @@
       <c r="J18" s="2">
         <v>5</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>0</v>
+      <c r="K18" s="2">
+        <v>5</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>0</v>
@@ -19367,8 +19541,8 @@
       <c r="J19" s="2">
         <v>4</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>0</v>
+      <c r="K19" s="2">
+        <v>5</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>0</v>
@@ -19635,8 +19809,8 @@
       <c r="J23" s="2">
         <v>5</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>0</v>
+      <c r="K23" s="2">
+        <v>5</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>0</v>
@@ -19703,8 +19877,8 @@
       <c r="J24" s="2">
         <v>5</v>
       </c>
-      <c r="K24" s="2" t="s">
-        <v>0</v>
+      <c r="K24" s="2">
+        <v>5</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>0</v>
@@ -19970,7 +20144,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20042,7 +20216,9 @@
       <c r="J5" s="7">
         <v>43438</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>43445</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -20086,8 +20262,8 @@
       <c r="J6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>0</v>
+      <c r="K6" s="2">
+        <v>7</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>0</v>
@@ -20154,8 +20330,8 @@
       <c r="J7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>0</v>
+      <c r="K7" s="2">
+        <v>3</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>0</v>
@@ -20210,8 +20386,8 @@
       <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>0</v>
+      <c r="G8" s="2">
+        <v>5</v>
       </c>
       <c r="H8" s="2">
         <v>5</v>
@@ -20222,8 +20398,8 @@
       <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>0</v>
+      <c r="K8" s="2">
+        <v>3</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>0</v>
@@ -20630,8 +20806,8 @@
       <c r="J14" s="2">
         <v>5</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>0</v>
+      <c r="K14" s="2">
+        <v>5</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
@@ -20830,8 +21006,8 @@
       <c r="J17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>0</v>
+      <c r="K17" s="2">
+        <v>5</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>0</v>
@@ -20898,8 +21074,8 @@
       <c r="J18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>0</v>
+      <c r="K18" s="2">
+        <v>5</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>0</v>
@@ -21103,7 +21279,7 @@
         <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>0</v>
@@ -21170,8 +21346,8 @@
       <c r="J22" s="2">
         <v>5</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>0</v>
+      <c r="K22" s="2">
+        <v>5</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>0</v>
@@ -21374,8 +21550,8 @@
       <c r="J25" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>0</v>
+      <c r="K25" s="2">
+        <v>5</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>0</v>
@@ -21510,8 +21686,8 @@
       <c r="J27" s="2">
         <v>4</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>0</v>
+      <c r="K27" s="2">
+        <v>5</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>0</v>
@@ -21749,7 +21925,7 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21818,7 +21994,9 @@
       <c r="J5" s="7">
         <v>43438</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>43445</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -21998,8 +22176,8 @@
       <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>0</v>
+      <c r="K8" s="2">
+        <v>5</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>0</v>
@@ -22335,11 +22513,11 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>0</v>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>5</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>0</v>
@@ -22474,8 +22652,8 @@
       <c r="J15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>0</v>
+      <c r="K15" s="2">
+        <v>5</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>0</v>
@@ -22930,26 +23108,26 @@
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>0</v>
+      <c r="E22" s="2">
+        <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>0</v>
@@ -23013,8 +23191,8 @@
       <c r="I23" s="2">
         <v>5</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>0</v>
+      <c r="J23" s="2">
+        <v>3</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>0</v>
@@ -23081,11 +23259,11 @@
       <c r="I24" s="2">
         <v>5</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>0</v>
+      <c r="J24" s="2">
+        <v>5</v>
+      </c>
+      <c r="K24" s="2">
+        <v>4</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>0</v>
@@ -23274,8 +23452,8 @@
       <c r="F27" s="2">
         <v>4</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>217</v>
+      <c r="G27" s="2">
+        <v>5</v>
       </c>
       <c r="H27" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
A fistful of labs
</commit_message>
<xml_diff>
--- a/register/2018.xlsx
+++ b/register/2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\nets\register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653B7912-3A87-4D3D-83C2-617DB7750D28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2CE44C-8654-4EAA-8867-7A0DFCA2316F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11715" activeTab="2" xr2:uid="{0773F02F-154F-49AB-B554-199499201140}"/>
   </bookViews>
@@ -377,6 +377,31 @@
     <author>С.С. Уколов</author>
   </authors>
   <commentList>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{A1A111B3-768E-46BA-B031-F032E57EA974}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+VLAN всё таки чужие ;-)
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K7" authorId="0" shapeId="0" xr:uid="{95598E74-3CF2-4CEE-B296-03695DC5D2D9}">
       <text>
         <r>
@@ -477,6 +502,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{4A0214D1-2C48-452C-876E-C21D129FD770}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Чужой IP
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L10" authorId="0" shapeId="0" xr:uid="{C78F6AD1-56BC-4A73-BD06-A744CB9648C5}">
       <text>
         <r>
@@ -522,54 +572,6 @@
           </rPr>
           <t xml:space="preserve">
 Не везде включён DHCP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{DAD6ED5C-DB19-4104-AF71-FB77F44C2962}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>С.С. Уколов:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Опечатки в таблицах маршрутизации</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L21" authorId="0" shapeId="0" xr:uid="{8F0356E2-22A0-4845-9EA9-B657D82A4091}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>С.С. Уколов:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Не точный DHCP-диапазон</t>
         </r>
       </text>
     </comment>
@@ -784,30 +786,6 @@
           <t xml:space="preserve">
 Маршрутизатор совсем не настроен
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{EDE0AB72-0393-43FB-B884-B38D58C2EC24}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>С.С. Уколов:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Чужие и разные (!) IP-адреса</t>
         </r>
       </text>
     </comment>
@@ -1049,7 +1027,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="226">
   <si>
     <t/>
   </si>
@@ -2288,7 +2266,7 @@
   <dimension ref="A1:XFD43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20287,7 +20265,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20398,8 +20376,8 @@
       <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>0</v>
+      <c r="H6" s="2">
+        <v>4</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>0</v>
@@ -20666,7 +20644,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>0</v>
@@ -20728,17 +20706,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
         <v>0</v>
       </c>
@@ -20748,8 +20724,8 @@
       <c r="K11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>0</v>
+      <c r="L11" s="2">
+        <v>5</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>0</v>
@@ -21214,8 +21190,8 @@
       <c r="I18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>216</v>
+      <c r="J18" s="2">
+        <v>5</v>
       </c>
       <c r="K18" s="2">
         <v>5</v>
@@ -21425,7 +21401,7 @@
         <v>5</v>
       </c>
       <c r="L21" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>0</v>
@@ -22067,8 +22043,8 @@
   </sheetPr>
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23322,7 +23298,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F23" s="2">
         <v>5</v>
@@ -23342,8 +23318,8 @@
       <c r="K23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>0</v>
+      <c r="L23" s="2">
+        <v>5</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
First & last labs
</commit_message>
<xml_diff>
--- a/register/2018.xlsx
+++ b/register/2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\nets\register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD6A633-AA08-4CA4-A7E7-4342130D3CA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF977DA8-C348-4851-9DA5-CC57E7D8B702}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11715" xr2:uid="{0773F02F-154F-49AB-B554-199499201140}"/>
   </bookViews>
@@ -314,6 +314,56 @@
           </rPr>
           <t xml:space="preserve">
 Не включен DHCP на рабочей станции</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{96AC883F-8023-4459-A990-52E5CB28E07B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Чужой IP
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{41AD757A-48FE-4CDA-AB2C-7F625C636398}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>С.С. Уколов:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Чужой IP
+</t>
         </r>
       </text>
     </comment>
@@ -2269,7 +2319,7 @@
   <dimension ref="A1:XFD43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19110,6 +19160,9 @@
       <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
       <c r="F11" s="2">
         <v>3</v>
       </c>
@@ -19874,10 +19927,10 @@
         <v>5</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>0</v>

</xml_diff>